<commit_message>
Add Baseball Salaries Excel File
Changed variable names to include underscores instead of spaces i.e. Home Runs changed to Home_Runs
</commit_message>
<xml_diff>
--- a/Baseball Salaries.xlsx
+++ b/Baseball Salaries.xlsx
@@ -1040,15 +1040,6 @@
     <t xml:space="preserve">Monty Fariss     </t>
   </si>
   <si>
-    <t>Player Name</t>
-  </si>
-  <si>
-    <t>Batting Average</t>
-  </si>
-  <si>
-    <t>On-Base Percentage</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -1064,40 +1055,49 @@
     <t>Triples</t>
   </si>
   <si>
-    <t>Home Runs</t>
-  </si>
-  <si>
     <t>RBIs</t>
   </si>
   <si>
     <t>Walks</t>
   </si>
   <si>
-    <t>Strike-Outs</t>
-  </si>
-  <si>
-    <t>Stolen Bases</t>
-  </si>
-  <si>
     <t>Errors</t>
   </si>
   <si>
-    <t>Free Agency Eligibility</t>
-  </si>
-  <si>
-    <t>Arbitration Elegibility</t>
-  </si>
-  <si>
-    <t>Slugging Percentage</t>
-  </si>
-  <si>
-    <t>Free Agent 1991/1992</t>
-  </si>
-  <si>
-    <t>Arbitration 1991/1992</t>
-  </si>
-  <si>
-    <t>Player ID</t>
+    <t>Player_ID</t>
+  </si>
+  <si>
+    <t>Player_Name</t>
+  </si>
+  <si>
+    <t>Batting_Average</t>
+  </si>
+  <si>
+    <t>OnBase_Percentage</t>
+  </si>
+  <si>
+    <t>Slugging_Percentage</t>
+  </si>
+  <si>
+    <t>Home_Runs</t>
+  </si>
+  <si>
+    <t>Strike_Outs</t>
+  </si>
+  <si>
+    <t>Stolen_Bases</t>
+  </si>
+  <si>
+    <t>Free_Agency_Eligibility</t>
+  </si>
+  <si>
+    <t>Free_Agent_1991/1992</t>
+  </si>
+  <si>
+    <t>Arbitration_Elegibility</t>
+  </si>
+  <si>
+    <t>Arbitration_1991/1992</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1105,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1149,7 +1149,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1433,7 +1433,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1462,64 +1462,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>351</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>354</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.25">

</xml_diff>